<commit_message>
adding column for recent count
</commit_message>
<xml_diff>
--- a/data/2025_AFDW_sorted.xlsx
+++ b/data/2025_AFDW_sorted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chloegilligan/Desktop/Repositories/Nucella_2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80BD3F4C-ECC5-8E4F-9A10-C0D331948F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E215BC1-88FA-F843-A17D-F7135923284F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{5273D207-4579-7847-A0D9-2C1FE3CF36B0}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" xr2:uid="{5273D207-4579-7847-A0D9-2C1FE3CF36B0}"/>
   </bookViews>
   <sheets>
     <sheet name="2025_AFDW_sorted" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="176">
   <si>
     <t>Tin..</t>
   </si>
@@ -539,6 +539,15 @@
   </si>
   <si>
     <t>Only one BRB6</t>
+  </si>
+  <si>
+    <t>Only one BRB3</t>
+  </si>
+  <si>
+    <t>Only one BRB1</t>
+  </si>
+  <si>
+    <t>Only one RIG2</t>
   </si>
 </sst>
 </file>
@@ -681,7 +690,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -867,6 +876,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1028,9 +1043,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1408,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8005B842-961A-9846-9D15-189B03AE4280}">
   <dimension ref="A1:L148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1468,33 +1484,36 @@
       <c r="H2">
         <v>20251020</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="K2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>141</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>208.51900000000001</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>0.19900000000000001</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>208.66300000000001</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>20251029</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>20251028</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1578,6 +1597,9 @@
       <c r="H6">
         <v>20251014</v>
       </c>
+      <c r="K6" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -1868,29 +1890,29 @@
         <v>20251028</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
         <v>20</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>206.893</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>0.193</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>207.06200000000001</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>20251006</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="2">
         <v>20251008</v>
       </c>
     </row>
@@ -1920,29 +1942,29 @@
         <v>20251014</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <v>52</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>206.87100000000001</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>0.20300000000000001</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>206.96899999999999</v>
       </c>
-      <c r="G20">
-        <v>20251014</v>
-      </c>
-      <c r="H20">
+      <c r="G20" s="2">
+        <v>20251014</v>
+      </c>
+      <c r="H20" s="2">
         <v>20251014</v>
       </c>
     </row>
@@ -3284,29 +3306,29 @@
         <v>20251028</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72">
+    <row r="72" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2">
         <v>51</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="2">
         <v>207.65</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="2">
         <v>0.32400000000000001</v>
       </c>
-      <c r="F72">
+      <c r="F72" s="2">
         <v>207.88800000000001</v>
       </c>
-      <c r="G72">
-        <v>20251014</v>
-      </c>
-      <c r="H72">
+      <c r="G72" s="2">
+        <v>20251014</v>
+      </c>
+      <c r="H72" s="2">
         <v>20251014</v>
       </c>
     </row>
@@ -3336,29 +3358,29 @@
         <v>20251014</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74">
+    <row r="74" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="2">
         <v>53</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="2">
         <v>207.636</v>
       </c>
-      <c r="E74">
+      <c r="E74" s="2">
         <v>0.23499999999999999</v>
       </c>
-      <c r="F74">
+      <c r="F74" s="2">
         <v>207.816</v>
       </c>
-      <c r="G74">
-        <v>20251014</v>
-      </c>
-      <c r="H74">
+      <c r="G74" s="2">
+        <v>20251014</v>
+      </c>
+      <c r="H74" s="2">
         <v>20251014</v>
       </c>
     </row>
@@ -3492,29 +3514,29 @@
         <v>20251020</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80">
+    <row r="80" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="2">
         <v>114</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="2">
         <v>210.50200000000001</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="2">
         <v>0.249</v>
       </c>
-      <c r="F80">
+      <c r="F80" s="2">
         <v>210.66800000000001</v>
       </c>
-      <c r="G80">
+      <c r="G80" s="2">
         <v>20251029</v>
       </c>
-      <c r="H80">
+      <c r="H80" s="2">
         <v>20251028</v>
       </c>
     </row>
@@ -3547,29 +3569,29 @@
         <v>169</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82">
+    <row r="82" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="2">
         <v>22</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="2">
         <v>207.65299999999999</v>
       </c>
-      <c r="E82">
+      <c r="E82" s="2">
         <v>0.20699999999999999</v>
       </c>
-      <c r="F82">
+      <c r="F82" s="2">
         <v>207.78800000000001</v>
       </c>
-      <c r="G82">
+      <c r="G82" s="2">
         <v>20251006</v>
       </c>
-      <c r="H82">
+      <c r="H82" s="2">
         <v>20251008</v>
       </c>
     </row>
@@ -3755,29 +3777,29 @@
         <v>20251028</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A90">
+    <row r="90" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="2">
         <v>29</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="2">
         <v>206.57</v>
       </c>
-      <c r="E90">
+      <c r="E90" s="2">
         <v>0.188</v>
       </c>
-      <c r="F90">
+      <c r="F90" s="2">
         <v>206.70500000000001</v>
       </c>
-      <c r="G90">
+      <c r="G90" s="2">
         <v>20251006</v>
       </c>
-      <c r="H90">
+      <c r="H90" s="2">
         <v>20251008</v>
       </c>
     </row>
@@ -3807,29 +3829,29 @@
         <v>20251008</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A92">
+    <row r="92" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="2">
         <v>108</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="2">
         <v>209.202</v>
       </c>
-      <c r="E92">
+      <c r="E92" s="2">
         <v>0.18</v>
       </c>
-      <c r="F92">
+      <c r="F92" s="2">
         <v>209.327</v>
       </c>
-      <c r="G92">
+      <c r="G92" s="2">
         <v>20251022</v>
       </c>
-      <c r="H92">
+      <c r="H92" s="2">
         <v>20251020</v>
       </c>
     </row>
@@ -3859,29 +3881,29 @@
         <v>20251020</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94">
+    <row r="94" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="2">
         <v>28</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="2">
         <v>207.709</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="2">
         <v>0.188</v>
       </c>
-      <c r="F94">
+      <c r="F94" s="2">
         <v>207.82</v>
       </c>
-      <c r="G94">
+      <c r="G94" s="2">
         <v>20251006</v>
       </c>
-      <c r="H94">
+      <c r="H94" s="2">
         <v>20251008</v>
       </c>
     </row>
@@ -3911,29 +3933,29 @@
         <v>20251020</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A96">
+    <row r="96" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="2">
         <v>150</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="2">
         <v>210.10900000000001</v>
       </c>
-      <c r="E96">
+      <c r="E96" s="2">
         <v>0.187</v>
       </c>
-      <c r="F96">
+      <c r="F96" s="2">
         <v>210.25</v>
       </c>
-      <c r="G96">
+      <c r="G96" s="2">
         <v>20251029</v>
       </c>
-      <c r="H96">
+      <c r="H96" s="2">
         <v>20251028</v>
       </c>
     </row>
@@ -4171,32 +4193,32 @@
         <v>20251014</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A106">
+    <row r="106" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="2">
         <v>18</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D106">
+      <c r="D106" s="2">
         <v>206.16399999999999</v>
       </c>
-      <c r="E106">
+      <c r="E106" s="2">
         <v>0.14099999999999999</v>
       </c>
-      <c r="F106">
+      <c r="F106" s="2">
         <v>206.26499999999999</v>
       </c>
-      <c r="G106">
+      <c r="G106" s="2">
         <v>20251006</v>
       </c>
-      <c r="H106">
+      <c r="H106" s="2">
         <v>20251008</v>
       </c>
-      <c r="I106" t="s">
+      <c r="I106" s="2" t="s">
         <v>119</v>
       </c>
     </row>
@@ -4226,29 +4248,29 @@
         <v>20251008</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A108">
+    <row r="108" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="2">
         <v>21</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D108">
+      <c r="D108" s="2">
         <v>206.489</v>
       </c>
-      <c r="E108">
+      <c r="E108" s="2">
         <v>0.19800000000000001</v>
       </c>
-      <c r="F108">
+      <c r="F108" s="2">
         <v>206.649</v>
       </c>
-      <c r="G108">
+      <c r="G108" s="2">
         <v>20251006</v>
       </c>
-      <c r="H108">
+      <c r="H108" s="2">
         <v>20251008</v>
       </c>
     </row>
@@ -4462,30 +4484,33 @@
       <c r="H116">
         <v>20251014</v>
       </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A117">
+      <c r="L116" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="2">
         <v>19</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D117">
+      <c r="D117" s="2">
         <v>208.005</v>
       </c>
-      <c r="E117">
+      <c r="E117" s="2">
         <v>0.111</v>
       </c>
-      <c r="F117">
+      <c r="F117" s="2">
         <v>208.095</v>
       </c>
-      <c r="G117">
+      <c r="G117" s="2">
         <v>20251006</v>
       </c>
-      <c r="H117">
+      <c r="H117" s="2">
         <v>20251008</v>
       </c>
     </row>
@@ -4518,29 +4543,29 @@
         <v>168</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A119">
+    <row r="119" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="2">
         <v>23</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D119">
+      <c r="D119" s="2">
         <v>206.17400000000001</v>
       </c>
-      <c r="E119">
+      <c r="E119" s="2">
         <v>0.154</v>
       </c>
-      <c r="F119">
+      <c r="F119" s="2">
         <v>206.29599999999999</v>
       </c>
-      <c r="G119">
+      <c r="G119" s="2">
         <v>20251006</v>
       </c>
-      <c r="H119">
+      <c r="H119" s="2">
         <v>20251008</v>
       </c>
     </row>
@@ -5047,29 +5072,29 @@
         <v>20251014</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A139">
+    <row r="139" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="2">
         <v>24</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C139" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D139">
+      <c r="D139" s="2">
         <v>208.20500000000001</v>
       </c>
-      <c r="E139">
+      <c r="E139" s="2">
         <v>0.19800000000000001</v>
       </c>
-      <c r="F139">
+      <c r="F139" s="2">
         <v>208.304</v>
       </c>
-      <c r="G139">
+      <c r="G139" s="2">
         <v>20251006</v>
       </c>
-      <c r="H139">
+      <c r="H139" s="2">
         <v>20251008</v>
       </c>
     </row>
@@ -5203,29 +5228,29 @@
         <v>20251014</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A145">
+    <row r="145" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="2">
         <v>54</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B145" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C145" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D145">
+      <c r="D145" s="2">
         <v>207.35300000000001</v>
       </c>
-      <c r="E145">
+      <c r="E145" s="2">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="F145">
+      <c r="F145" s="2">
         <v>207.38</v>
       </c>
-      <c r="G145">
-        <v>20251014</v>
-      </c>
-      <c r="H145">
+      <c r="G145" s="2">
+        <v>20251014</v>
+      </c>
+      <c r="H145" s="2">
         <v>20251014</v>
       </c>
     </row>

</xml_diff>